<commit_message>
pcb v1.6. new rj45 footprint. swapped W49 and W51 so now interrupt vector 13 is on DIO_C of port 2. can have entire row of DIO-A and DIO-B interrupts without collisions
</commit_message>
<xml_diff>
--- a/pcb/bom/bom.xlsx
+++ b/pcb/bom/bom.xlsx
@@ -14,20 +14,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
-  <si>
-    <t>Ref</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Qty</t>
   </si>
   <si>
-    <t>Value</t>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Value/MPN</t>
   </si>
   <si>
     <t>Purchase Link</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>C2, C1</t>
   </si>
   <si>
@@ -58,28 +70,19 @@
     <t>X2U1, X1U1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>10µF (1206)</t>
+    <t>1206 Capacitor</t>
   </si>
   <si>
     <t>Schottky Diode</t>
   </si>
   <si>
-    <t>MicroUSB Connector</t>
-  </si>
-  <si>
-    <t>12-port RJ45</t>
-  </si>
-  <si>
-    <t>Barrel Jack</t>
+    <t>Micro USB Socket</t>
+  </si>
+  <si>
+    <t>12-port RJ45 Connector</t>
+  </si>
+  <si>
+    <t>Barrel Jack Connector</t>
   </si>
   <si>
     <t>Large Tactile Switch</t>
@@ -88,13 +91,43 @@
     <t>Small Tactile Switch</t>
   </si>
   <si>
-    <t>Voltage Regulator</t>
+    <t>5V DC to DC Converter</t>
+  </si>
+  <si>
+    <t>8-channel Driver Array</t>
+  </si>
+  <si>
+    <t>40-pin Connector</t>
+  </si>
+  <si>
+    <t>10µF</t>
+  </si>
+  <si>
+    <t>MBR120VLSFT3G</t>
+  </si>
+  <si>
+    <t>10118194-0001LF</t>
+  </si>
+  <si>
+    <t>5569263-1</t>
+  </si>
+  <si>
+    <t>PJ-037A</t>
+  </si>
+  <si>
+    <t>TL3300DF160Q</t>
+  </si>
+  <si>
+    <t>B3FS-1010P</t>
+  </si>
+  <si>
+    <t>R-78E5.0-1.0</t>
   </si>
   <si>
     <t>TBD62083A</t>
   </si>
   <si>
-    <t>40-pin Connector</t>
+    <t>DF40HC(4.0)-40DS-0.4V(70)</t>
   </si>
   <si>
     <t>https://www.digikey.com/products/en?keywords=1276-1804-1-ND</t>
@@ -115,7 +148,7 @@
     <t>https://www.digikey.com/products/en?keywords=EG4906CT-ND</t>
   </si>
   <si>
-    <t>https://omronfs.omron.com/en_US/ecb/products/pdf/en-b3f.pdf</t>
+    <t>https://www.digikey.com/products/en?keywords=sw1440ct</t>
   </si>
   <si>
     <t>https://www.digikey.com/products/en?keywords=945-2201-ND</t>
@@ -495,13 +528,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,159 +547,192 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
-    <hyperlink ref="D9" r:id="rId8"/>
-    <hyperlink ref="D10" r:id="rId9"/>
-    <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>